<commit_message>
Places the student correctly with OOP
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -22,7 +22,7 @@
     <t>FirstName</t>
   </si>
   <si>
-    <t>MidleName</t>
+    <t>MiddleName</t>
   </si>
   <si>
     <t>FamilyName</t>
@@ -1083,7 +1083,7 @@
         <v>3.4</v>
       </c>
       <c r="U2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -1139,7 +1139,7 @@
         <v>2.2</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1201,7 +1201,7 @@
         <v>3.2</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1257,7 +1257,7 @@
         <v>2.4</v>
       </c>
       <c r="U5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1313,7 +1313,7 @@
         <v>3.4</v>
       </c>
       <c r="U6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1431,7 +1431,7 @@
         <v>2.9</v>
       </c>
       <c r="U8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1490,7 +1490,7 @@
         <v>3</v>
       </c>
       <c r="U9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1546,7 +1546,7 @@
         <v>2.2</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1602,7 +1602,7 @@
         <v>2.3</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1717,7 +1717,7 @@
         <v>2</v>
       </c>
       <c r="U13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1776,7 +1776,7 @@
         <v>2.65</v>
       </c>
       <c r="U14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1832,7 +1832,7 @@
         <v>3</v>
       </c>
       <c r="U15">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1888,7 +1888,7 @@
         <v>2.4</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1944,7 +1944,7 @@
         <v>2.8</v>
       </c>
       <c r="U17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -2056,7 +2056,7 @@
         <v>2.8</v>
       </c>
       <c r="U19">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -2118,7 +2118,7 @@
         <v>2.7</v>
       </c>
       <c r="U20">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -2236,7 +2236,7 @@
         <v>2.9</v>
       </c>
       <c r="U22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -2292,7 +2292,7 @@
         <v>3.8</v>
       </c>
       <c r="U23">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -2410,7 +2410,7 @@
         <v>4</v>
       </c>
       <c r="U25">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -2522,7 +2522,7 @@
         <v>2</v>
       </c>
       <c r="U27">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -2578,7 +2578,7 @@
         <v>3.4</v>
       </c>
       <c r="U28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -2690,7 +2690,7 @@
         <v>2.4</v>
       </c>
       <c r="U30">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -2749,7 +2749,7 @@
         <v>2</v>
       </c>
       <c r="U31">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -2808,7 +2808,7 @@
         <v>2.65</v>
       </c>
       <c r="U32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -2920,7 +2920,7 @@
         <v>2.6</v>
       </c>
       <c r="U34">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:21">
@@ -3032,7 +3032,7 @@
         <v>3.2</v>
       </c>
       <c r="U36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -3147,7 +3147,7 @@
         <v>2.3</v>
       </c>
       <c r="U38">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -3203,7 +3203,7 @@
         <v>4.4</v>
       </c>
       <c r="U39">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -3262,7 +3262,7 @@
         <v>2.9</v>
       </c>
       <c r="U40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -3377,7 +3377,7 @@
         <v>2.5</v>
       </c>
       <c r="U42">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -3436,7 +3436,7 @@
         <v>2.266666666666667</v>
       </c>
       <c r="U43">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -3492,7 +3492,7 @@
         <v>2.8</v>
       </c>
       <c r="U44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -3551,7 +3551,7 @@
         <v>2.266666666666667</v>
       </c>
       <c r="U45">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -3607,7 +3607,7 @@
         <v>2.8</v>
       </c>
       <c r="U46">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -3725,7 +3725,7 @@
         <v>2.5</v>
       </c>
       <c r="U48">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -3784,7 +3784,7 @@
         <v>3.8</v>
       </c>
       <c r="U49">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -3840,7 +3840,7 @@
         <v>3.6</v>
       </c>
       <c r="U50">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -4011,7 +4011,7 @@
         <v>2.4</v>
       </c>
       <c r="U53">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -4123,7 +4123,7 @@
         <v>3</v>
       </c>
       <c r="U55">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -4179,7 +4179,7 @@
         <v>4.2</v>
       </c>
       <c r="U56">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -4235,7 +4235,7 @@
         <v>2.866666666666667</v>
       </c>
       <c r="U57">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -4350,7 +4350,7 @@
         <v>2.6</v>
       </c>
       <c r="U59">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:21">
@@ -4406,7 +4406,7 @@
         <v>2.6</v>
       </c>
       <c r="U60">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:21">
@@ -4524,7 +4524,7 @@
         <v>3.4</v>
       </c>
       <c r="U62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -4580,7 +4580,7 @@
         <v>3.2</v>
       </c>
       <c r="U63">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:21">
@@ -4636,7 +4636,7 @@
         <v>3.3</v>
       </c>
       <c r="U64">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:21">
@@ -4748,7 +4748,7 @@
         <v>3.8</v>
       </c>
       <c r="U66">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:21">
@@ -4807,7 +4807,7 @@
         <v>2.4</v>
       </c>
       <c r="U67">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:21">
@@ -4863,7 +4863,7 @@
         <v>2.4</v>
       </c>
       <c r="U68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:21">
@@ -4919,7 +4919,7 @@
         <v>3.4</v>
       </c>
       <c r="U69">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:21">
@@ -4975,7 +4975,7 @@
         <v>2.65</v>
       </c>
       <c r="U70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:21">
@@ -5031,7 +5031,7 @@
         <v>2.4</v>
       </c>
       <c r="U71">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:21">
@@ -5090,7 +5090,7 @@
         <v>2</v>
       </c>
       <c r="U72">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:21">
@@ -5146,7 +5146,7 @@
         <v>3.2</v>
       </c>
       <c r="U73">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:21">
@@ -5205,7 +5205,7 @@
         <v>2.65</v>
       </c>
       <c r="U74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:21">
@@ -5261,7 +5261,7 @@
         <v>3</v>
       </c>
       <c r="U75">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:21">
@@ -5320,7 +5320,7 @@
         <v>3.4</v>
       </c>
       <c r="U76">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:21">
@@ -5379,7 +5379,7 @@
         <v>3.3</v>
       </c>
       <c r="U77">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:21">
@@ -5435,7 +5435,7 @@
         <v>3.6</v>
       </c>
       <c r="U78">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:21">
@@ -5491,7 +5491,7 @@
         <v>3.2</v>
       </c>
       <c r="U79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:21">
@@ -5547,7 +5547,7 @@
         <v>3.2</v>
       </c>
       <c r="U80">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:21">
@@ -5603,7 +5603,7 @@
         <v>2.266666666666667</v>
       </c>
       <c r="U81">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:21">
@@ -5774,7 +5774,7 @@
         <v>3</v>
       </c>
       <c r="U84">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:21">
@@ -5830,7 +5830,7 @@
         <v>2.6</v>
       </c>
       <c r="U85">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:21">
@@ -5886,7 +5886,7 @@
         <v>2.4</v>
       </c>
       <c r="U86">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:21">
@@ -5945,7 +5945,7 @@
         <v>2.4</v>
       </c>
       <c r="U87">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:21">
@@ -6004,7 +6004,7 @@
         <v>2.6</v>
       </c>
       <c r="U88">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:21">
@@ -6060,7 +6060,7 @@
         <v>2.9</v>
       </c>
       <c r="U89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:21">
@@ -6116,7 +6116,7 @@
         <v>3.2</v>
       </c>
       <c r="U90">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:21">
@@ -6175,7 +6175,7 @@
         <v>2.9</v>
       </c>
       <c r="U91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:21">
@@ -6231,7 +6231,7 @@
         <v>3.4</v>
       </c>
       <c r="U92">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:21">
@@ -6287,7 +6287,7 @@
         <v>2.7</v>
       </c>
       <c r="U93">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:21">
@@ -6346,7 +6346,7 @@
         <v>2.9</v>
       </c>
       <c r="U94">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:21">
@@ -6464,7 +6464,7 @@
         <v>2.866666666666667</v>
       </c>
       <c r="U96">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:21">
@@ -6520,7 +6520,7 @@
         <v>3</v>
       </c>
       <c r="U97">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:21">
@@ -6632,7 +6632,7 @@
         <v>2.2</v>
       </c>
       <c r="U99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:21">
@@ -6691,7 +6691,7 @@
         <v>2.866666666666667</v>
       </c>
       <c r="U100">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>